<commit_message>
Serialization and De-serialization Concepts
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intellij-projects\API_Testing_Poudhan\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7A460D-5A66-48D3-9186-790C9CA95CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901B60E7-E2FF-4F17-AF3C-6DFCCA75BBAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login_credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>userid</t>
   </si>
@@ -43,16 +43,51 @@
   </si>
   <si>
     <t>pass2</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>sid@test.com</t>
+  </si>
+  <si>
+    <t>poudhan@test.com</t>
+  </si>
+  <si>
+    <t>2132138098</t>
+  </si>
+  <si>
+    <t>32840932</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +110,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,39 +399,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6BD79A65-CA26-468A-9994-D6BF91FBEA1D}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{0265BDEC-7602-402E-A2FE-FC994E33ABAB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>